<commit_message>
with IFLT pngs added, folder structure updated
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/experiment-data/1 - math/no iflt/22-30-02/data.xlsx
+++ b/GeneticProgrammingPortfolio/experiment-data/1 - math/no iflt/22-30-02/data.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\experiment-data\exp-1\no iflt\22-30-02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\experiment-data\1 - math\no iflt\22-30-02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11910" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Math, No IFLT" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Entire Ensemble in Testing" sheetId="2" r:id="rId1"/>
+    <sheet name="Individual Models in Testing" sheetId="4" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>DJIA</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Data Deleted: 35</t>
+  </si>
+  <si>
+    <t>BEST_IND(11)</t>
+  </si>
+  <si>
+    <t>AVG_IND(18)</t>
   </si>
 </sst>
 </file>
@@ -139,7 +146,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Math, No IFLT</a:t>
+              <a:t>Ensemble</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Testing Average &amp; Median (No IFLT)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1784,7 +1795,1146 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Best &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Average Individual from Ensemble (No IFLT)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DJIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.84026811000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83498734399999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85444194600000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86634980399999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86080725199999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83614498199999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84682125600000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83154587999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82724681099999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.820568721</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83020295200000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.80361808499999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.80763326899999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.82765563900000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82657704700000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.84360672999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86945043700000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87061997400000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.88099791400000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.89276637999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.89563412499999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.89966035799999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.89541313700000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.88205695699999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.90050096300000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.90680932299999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.90804770599999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.90690621800000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.90278393999999995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93002922099999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94341940000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.94140925799999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93787174900000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.95470849099999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.95269239999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.94485072299999995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.95889366600000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.96649140600000005</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.96219318799999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96184045699999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96582674199999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.950540316</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.95289723900000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.94813834500000005</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.92653675999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.90929713899999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.92950650000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.93005811999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.95110808499999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.95073325500000005</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.958472938</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.95582703099999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.95748529199999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.95758728599999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.956320854</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.94964276400000003</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.96395854299999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.95047232000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.92905262399999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.96049752899999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.95054286600000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.93673026000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.93029610699999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.93730397899999995</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.91099449700000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.91977367399999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.933067808</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.95212208099999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.93059699100000004</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89937902300000006</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.90983941000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.92391890099999996</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.93967195199999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.93538478300000005</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.933353392</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94973285900000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.93977904599999995</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.92457846499999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C84-48E4-8DB2-9BC2FCF7FA52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG_IND(18)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$2:$M$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.90339533334281397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90529991560145195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90733928501784999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90954197816189897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92955081826554098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92982260986110699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92939006587181505</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92825130722675098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92651699421340505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92441292055108304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.92225590564496895</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.92039786655077904</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91914299017332501</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91865824952585995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91890840979256805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.91964381869084999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.92045083033998398</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.92084991735230504</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92041034391551102</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.91885139304500096</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.91611294738462101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.912388621745299</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.90811537149513599</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90391147439180197</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.90046152283626801</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.898364528075974</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.89797998405871304</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.89931573510163298</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.90199593142054801</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.90532813982434701</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.90846020333684496</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.91058957187739897</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.91117465807023401</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.91010270771104196</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.90777131836186498</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.90502434794319098</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.90288664846960298</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.902134950753262</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.90289797364590996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.90453799680468105</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.90591456735528397</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.905881332773253</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.90375482719797395</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.89958507225708795</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.89418578615412703</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.88892248532579798</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.88528242171057803</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.88433928077271995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.88631457565121097</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.89043435725768905</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.89517246082384605</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.89880732991740997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.90008295616079503</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.89873908029355098</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.89571279700096096</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.89280206477551605</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.89171017389266405</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89291791801602005</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.89526401545345002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.89665606355629401</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.89535195908653797</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.89093344800454499</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.88456843112002004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.87855877587003905</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.87531699504610605</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.87617387054636098</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.88063323294587303</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.88653289150016001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.89109109553223498</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89232035727759096</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.89012478751900603</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.886501042833306</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.88436596152521296</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.88532010873896705</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.888174116456105</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.88985600194064896</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.88783509961768803</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.88193239489415998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9C84-48E4-8DB2-9BC2FCF7FA52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BEST_IND(11)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$2:$N$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.90270088120030201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90328122712829495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90386122070634001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90225773498971296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90264675524217997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90542864992687899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90617740867741003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90675543459270302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90733302395936499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90635874928929705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90602414034979295</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90817950430361905</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90963875689318496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91021396905204799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.910788667251481</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.91051032697619305</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.90960803715683802</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.91106856512258305</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.91308208544663705</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.91365403856229799</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.91422540798705898</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.91464466308615699</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91335933754780196</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.91412312393457795</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.91650483752543099</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.91707313329006601</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.91764078198908805</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.91820777494981298</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.91722716934416804</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.91735228335867902</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.91947529065774103</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.92046901055151098</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.92103258961825596</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.92159545901361395</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.92115509388614503</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.920747343034652</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.922327231017678</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.92383967916819199</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.92439888009257398</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.92495732368619898</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.92508689630802299</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.92428413048689195</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.92529242857432203</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.92718338344196205</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.92773793549511796</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.92829168843554599</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.92884463208093904</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.92792681561942902</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.92838594951169195</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.93040886777395204</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.93104825476646402</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.93159708683136599</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.93214507833068505</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.93163252121187801</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.93160838736825702</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.93321820942862799</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.93432853790681103</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.93487225089120196</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.93541509328091899</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.935356006046143</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.93494698580775104</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.936098434435786</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.93757767055716201</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.93811609576483102</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.93865362492934801</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.93905382886461697</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.93837805950337505</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.93906803507841496</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.94079470886383798</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.94132770495403495</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.94185978348701804</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.94239094161375903</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.94187028566589404</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.94213394286056995</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.94371141051799201</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94450631616952896</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.94503283105618197</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.94555840906209299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9C84-48E4-8DB2-9BC2FCF7FA52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="475380992"/>
+        <c:axId val="475385912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="475380992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475385912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="475385912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.05"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475380992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2340,6 +3490,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -2351,7 +4017,45 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2663,15 +4367,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M1" activeCellId="1" sqref="A1:A79 M1:N79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2702,8 +4406,14 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.84026811000000001</v>
       </c>
@@ -2735,8 +4445,14 @@
         <f>SUM(G2:G79)</f>
         <v>0.20098174188174689</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0.90339533334281397</v>
+      </c>
+      <c r="N2">
+        <v>0.90270088120030201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.83498734399999996</v>
       </c>
@@ -2760,8 +4476,14 @@
         <f t="shared" si="1"/>
         <v>8.0199081288351848E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0.90529991560145195</v>
+      </c>
+      <c r="N3">
+        <v>0.90328122712829495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.85444194600000001</v>
       </c>
@@ -2785,8 +4507,14 @@
         <f t="shared" si="1"/>
         <v>4.9111391409061289E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0.90733928501784999</v>
+      </c>
+      <c r="N4">
+        <v>0.90386122070634001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.86634980399999995</v>
       </c>
@@ -2810,8 +4538,14 @@
         <f t="shared" si="1"/>
         <v>3.3815936199013464E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0.90954197816189897</v>
+      </c>
+      <c r="N5">
+        <v>0.90225773498971296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.86080725199999997</v>
       </c>
@@ -2835,8 +4569,14 @@
         <f t="shared" si="1"/>
         <v>4.7256779029048431E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0.92955081826554098</v>
+      </c>
+      <c r="N6">
+        <v>0.90264675524217997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.83614498199999998</v>
       </c>
@@ -2860,8 +4600,14 @@
         <f t="shared" si="1"/>
         <v>8.775497961684052E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0.92982260986110699</v>
+      </c>
+      <c r="N7">
+        <v>0.90542864992687899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.84682125600000002</v>
       </c>
@@ -2885,8 +4631,14 @@
         <f t="shared" si="1"/>
         <v>6.8176083636480121E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0.92939006587181505</v>
+      </c>
+      <c r="N8">
+        <v>0.90617740867741003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.83154587999999996</v>
       </c>
@@ -2910,8 +4662,14 @@
         <f t="shared" si="1"/>
         <v>1.1283697048386934E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0.92825130722675098</v>
+      </c>
+      <c r="N9">
+        <v>0.90675543459270302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.82724681099999997</v>
       </c>
@@ -2935,8 +4693,14 @@
         <f t="shared" si="1"/>
         <v>1.2271234915567454E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0.92651699421340505</v>
+      </c>
+      <c r="N10">
+        <v>0.90733302395936499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.820568721</v>
       </c>
@@ -2960,8 +4724,14 @@
         <f t="shared" si="1"/>
         <v>1.381125081130264E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0.92441292055108304</v>
+      </c>
+      <c r="N11">
+        <v>0.90635874928929705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.83020295200000005</v>
       </c>
@@ -2985,8 +4755,14 @@
         <f t="shared" si="1"/>
         <v>8.8636006937253091E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0.92225590564496895</v>
+      </c>
+      <c r="N12">
+        <v>0.90602414034979295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.80361808499999998</v>
       </c>
@@ -3010,8 +4786,14 @@
         <f t="shared" si="1"/>
         <v>1.4570531520677688E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.92039786655077904</v>
+      </c>
+      <c r="N13">
+        <v>0.90817950430361905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.80763326899999999</v>
       </c>
@@ -3035,8 +4817,14 @@
         <f t="shared" si="1"/>
         <v>1.3611844249402644E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0.91914299017332501</v>
+      </c>
+      <c r="N14">
+        <v>0.90963875689318496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.82765563900000005</v>
       </c>
@@ -3060,8 +4848,14 @@
         <f t="shared" si="1"/>
         <v>1.2254830452479902E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0.91865824952585995</v>
+      </c>
+      <c r="N15">
+        <v>0.91021396905204799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.82657704700000001</v>
       </c>
@@ -3085,8 +4879,14 @@
         <f t="shared" si="1"/>
         <v>1.250955996844451E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0.91890840979256805</v>
+      </c>
+      <c r="N16">
+        <v>0.910788667251481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.84360672999999997</v>
       </c>
@@ -3110,8 +4910,14 @@
         <f t="shared" si="1"/>
         <v>9.0026255577669509E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0.91964381869084999</v>
+      </c>
+      <c r="N17">
+        <v>0.91051032697619305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.86945043700000002</v>
       </c>
@@ -3135,8 +4941,14 @@
         <f t="shared" si="1"/>
         <v>4.77534315767905E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0.92045083033998398</v>
+      </c>
+      <c r="N18">
+        <v>0.90960803715683802</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.87061997400000002</v>
       </c>
@@ -3160,8 +4972,14 @@
         <f t="shared" si="1"/>
         <v>4.6239201481680578E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0.92084991735230504</v>
+      </c>
+      <c r="N19">
+        <v>0.91106856512258305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.88099791400000005</v>
       </c>
@@ -3185,8 +5003,14 @@
         <f t="shared" si="1"/>
         <v>3.3277046435262014E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0.92041034391551102</v>
+      </c>
+      <c r="N20">
+        <v>0.91308208544663705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.89276637999999997</v>
       </c>
@@ -3210,8 +5034,14 @@
         <f t="shared" si="1"/>
         <v>2.1143699810339603E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0.91885139304500096</v>
+      </c>
+      <c r="N21">
+        <v>0.91365403856229799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.89563412499999995</v>
       </c>
@@ -3235,8 +5065,14 @@
         <f t="shared" si="1"/>
         <v>1.864401597583429E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>0.91611294738462101</v>
+      </c>
+      <c r="N22">
+        <v>0.91422540798705898</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.89966035799999999</v>
       </c>
@@ -3260,8 +5096,14 @@
         <f t="shared" si="1"/>
         <v>1.5379234225507989E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>0.912388621745299</v>
+      </c>
+      <c r="N23">
+        <v>0.91464466308615699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.89541313700000003</v>
       </c>
@@ -3285,8 +5127,14 @@
         <f t="shared" si="1"/>
         <v>1.8826190040447585E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>0.90811537149513599</v>
+      </c>
+      <c r="N24">
+        <v>0.91335933754780196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.88205695699999997</v>
       </c>
@@ -3310,8 +5158,14 @@
         <f t="shared" si="1"/>
         <v>2.7606650712807619E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>0.90391147439180197</v>
+      </c>
+      <c r="N25">
+        <v>0.91412312393457795</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.90050096300000004</v>
       </c>
@@ -3335,8 +5189,14 @@
         <f t="shared" si="1"/>
         <v>1.1629313389548469E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>0.90046152283626801</v>
+      </c>
+      <c r="N26">
+        <v>0.91650483752543099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.90680932299999994</v>
       </c>
@@ -3360,8 +5220,14 @@
         <f t="shared" si="1"/>
         <v>7.6682015054791038E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>0.898364528075974</v>
+      </c>
+      <c r="N27">
+        <v>0.91707313329006601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.90804770599999995</v>
       </c>
@@ -3385,8 +5251,14 @@
         <f t="shared" si="1"/>
         <v>5.137239572421304E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>0.89797998405871304</v>
+      </c>
+      <c r="N28">
+        <v>0.91764078198908805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.90690621800000004</v>
       </c>
@@ -3410,8 +5282,14 @@
         <f t="shared" si="1"/>
         <v>6.153709223469517E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>0.89931573510163298</v>
+      </c>
+      <c r="N29">
+        <v>0.91820777494981298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.90278393999999995</v>
       </c>
@@ -3435,8 +5313,14 @@
         <f t="shared" si="1"/>
         <v>9.4984042370468069E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>0.90199593142054801</v>
+      </c>
+      <c r="N30">
+        <v>0.91722716934416804</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.93002922099999996</v>
       </c>
@@ -3460,8 +5344,14 @@
         <f t="shared" si="1"/>
         <v>1.0064178824765196E-5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>0.90532813982434701</v>
+      </c>
+      <c r="N31">
+        <v>0.91735228335867902</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.94341940000000002</v>
       </c>
@@ -3485,8 +5375,14 @@
         <f t="shared" si="1"/>
         <v>1.1380550075209323E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>0.90846020333684496</v>
+      </c>
+      <c r="N32">
+        <v>0.91947529065774103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.94140925799999997</v>
       </c>
@@ -3510,8 +5406,14 @@
         <f t="shared" si="1"/>
         <v>2.3617172839549932E-4</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>0.91058957187739897</v>
+      </c>
+      <c r="N33">
+        <v>0.92046901055151098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.93787174900000003</v>
       </c>
@@ -3535,8 +5437,14 @@
         <f t="shared" ref="G34:G65" si="3">ABS(C34-A34)^2</f>
         <v>1.4889802046455671E-4</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>0.91117465807023401</v>
+      </c>
+      <c r="N34">
+        <v>0.92103258961825596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.95470849099999999</v>
       </c>
@@ -3560,8 +5468,14 @@
         <f t="shared" si="3"/>
         <v>8.6758163461713594E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>0.91010270771104196</v>
+      </c>
+      <c r="N35">
+        <v>0.92159545901361395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.95269239999999999</v>
       </c>
@@ -3585,8 +5499,14 @@
         <f t="shared" si="3"/>
         <v>4.9254523353475712E-4</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>0.90777131836186498</v>
+      </c>
+      <c r="N36">
+        <v>0.92115509388614503</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.94485072299999995</v>
       </c>
@@ -3610,8 +5530,14 @@
         <f t="shared" si="3"/>
         <v>4.224054938819625E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>0.90502434794319098</v>
+      </c>
+      <c r="N37">
+        <v>0.920747343034652</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.95889366600000003</v>
       </c>
@@ -3635,8 +5561,14 @@
         <f t="shared" si="3"/>
         <v>1.2342422747843385E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>0.90288664846960298</v>
+      </c>
+      <c r="N38">
+        <v>0.922327231017678</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.96649140600000005</v>
       </c>
@@ -3660,8 +5592,14 @@
         <f t="shared" si="3"/>
         <v>1.4117808875079424E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>0.902134950753262</v>
+      </c>
+      <c r="N39">
+        <v>0.92383967916819199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.96219318799999998</v>
       </c>
@@ -3685,8 +5623,14 @@
         <f t="shared" si="3"/>
         <v>1.1009468897009351E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>0.90289797364590996</v>
+      </c>
+      <c r="N40">
+        <v>0.92439888009257398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.96184045699999998</v>
       </c>
@@ -3710,8 +5654,14 @@
         <f t="shared" si="3"/>
         <v>1.0714409491085386E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>0.90453799680468105</v>
+      </c>
+      <c r="N41">
+        <v>0.92495732368619898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.96582674199999996</v>
       </c>
@@ -3735,8 +5685,14 @@
         <f t="shared" si="3"/>
         <v>1.7246193184554464E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>0.90591456735528397</v>
+      </c>
+      <c r="N42">
+        <v>0.92508689630802299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.950540316</v>
       </c>
@@ -3760,8 +5716,14 @@
         <f t="shared" si="3"/>
         <v>7.1075342499421653E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>0.905881332773253</v>
+      </c>
+      <c r="N43">
+        <v>0.92428413048689195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.95289723900000001</v>
       </c>
@@ -3785,8 +5747,14 @@
         <f t="shared" si="3"/>
         <v>8.1392368041993365E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>0.90375482719797395</v>
+      </c>
+      <c r="N44">
+        <v>0.92529242857432203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.94813834500000005</v>
       </c>
@@ -3810,8 +5778,14 @@
         <f t="shared" si="3"/>
         <v>5.2174500711343495E-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>0.89958507225708795</v>
+      </c>
+      <c r="N45">
+        <v>0.92718338344196205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.92653675999999996</v>
       </c>
@@ -3835,8 +5809,14 @@
         <f t="shared" si="3"/>
         <v>2.1887990942287497E-6</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>0.89418578615412703</v>
+      </c>
+      <c r="N46">
+        <v>0.92773793549511796</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.90929713899999998</v>
       </c>
@@ -3860,8 +5840,14 @@
         <f t="shared" si="3"/>
         <v>4.1548597249738823E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>0.88892248532579798</v>
+      </c>
+      <c r="N47">
+        <v>0.92829168843554599</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.92950650000000001</v>
       </c>
@@ -3885,8 +5871,14 @@
         <f t="shared" si="3"/>
         <v>7.3354204777614172E-8</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>0.88528242171057803</v>
+      </c>
+      <c r="N48">
+        <v>0.92884463208093904</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.93005811999999999</v>
       </c>
@@ -3910,8 +5902,14 @@
         <f t="shared" si="3"/>
         <v>8.436435645358105E-7</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>0.88433928077271995</v>
+      </c>
+      <c r="N49">
+        <v>0.92792681561942902</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.95110808499999999</v>
       </c>
@@ -3935,8 +5933,14 @@
         <f t="shared" si="3"/>
         <v>4.803423043896607E-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>0.88631457565121097</v>
+      </c>
+      <c r="N50">
+        <v>0.92838594951169195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.95073325500000005</v>
       </c>
@@ -3960,8 +5964,14 @@
         <f t="shared" si="3"/>
         <v>4.2878708336292889E-4</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>0.89043435725768905</v>
+      </c>
+      <c r="N51">
+        <v>0.93040886777395204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.958472938</v>
       </c>
@@ -3985,8 +5995,14 @@
         <f t="shared" si="3"/>
         <v>8.0104782440172206E-4</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>0.89517246082384605</v>
+      </c>
+      <c r="N52">
+        <v>0.93104825476646402</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.95582703099999999</v>
       </c>
@@ -4010,8 +6026,14 @@
         <f t="shared" si="3"/>
         <v>6.5315515953254548E-4</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>0.89880732991740997</v>
+      </c>
+      <c r="N53">
+        <v>0.93159708683136599</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.95748529199999999</v>
       </c>
@@ -4035,8 +6057,14 @@
         <f t="shared" si="3"/>
         <v>7.3518805350595347E-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>0.90008295616079503</v>
+      </c>
+      <c r="N54">
+        <v>0.93214507833068505</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.95758728599999998</v>
       </c>
@@ -4060,8 +6088,14 @@
         <f t="shared" si="3"/>
         <v>7.6421845862536804E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <v>0.89873908029355098</v>
+      </c>
+      <c r="N55">
+        <v>0.93163252121187801</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.956320854</v>
       </c>
@@ -4085,8 +6119,14 @@
         <f t="shared" si="3"/>
         <v>7.0546803415990483E-4</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <v>0.89571279700096096</v>
+      </c>
+      <c r="N56">
+        <v>0.93160838736825702</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.94964276400000003</v>
       </c>
@@ -4110,8 +6150,14 @@
         <f t="shared" si="3"/>
         <v>3.7043692538941037E-4</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>0.89280206477551605</v>
+      </c>
+      <c r="N57">
+        <v>0.93321820942862799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.96395854299999995</v>
       </c>
@@ -4135,8 +6181,14 @@
         <f t="shared" si="3"/>
         <v>1.1005785608780468E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>0.89171017389266405</v>
+      </c>
+      <c r="N58">
+        <v>0.93432853790681103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.95047232000000004</v>
       </c>
@@ -4160,8 +6212,14 @@
         <f t="shared" si="3"/>
         <v>3.834930582408948E-4</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <v>0.89291791801602005</v>
+      </c>
+      <c r="N59">
+        <v>0.93487225089120196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0.92905262399999999</v>
       </c>
@@ -4185,8 +6243,14 @@
         <f t="shared" si="3"/>
         <v>2.8595508460623542E-6</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <v>0.89526401545345002</v>
+      </c>
+      <c r="N60">
+        <v>0.93541509328091899</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.96049752899999996</v>
       </c>
@@ -4210,8 +6274,14 @@
         <f t="shared" si="3"/>
         <v>8.9874396631984903E-4</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <v>0.89665606355629401</v>
+      </c>
+      <c r="N61">
+        <v>0.935356006046143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.95054286600000004</v>
       </c>
@@ -4235,8 +6305,14 @@
         <f t="shared" si="3"/>
         <v>4.0999428768463263E-4</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <v>0.89535195908653797</v>
+      </c>
+      <c r="N62">
+        <v>0.93494698580775104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.93673026000000004</v>
       </c>
@@ -4260,8 +6336,14 @@
         <f t="shared" si="3"/>
         <v>4.4328886468894024E-5</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <v>0.89093344800454499</v>
+      </c>
+      <c r="N63">
+        <v>0.936098434435786</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.93029610699999998</v>
       </c>
@@ -4285,8 +6367,14 @@
         <f t="shared" si="3"/>
         <v>1.9753028019856806E-7</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>0.88456843112002004</v>
+      </c>
+      <c r="N64">
+        <v>0.93757767055716201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.93730397899999995</v>
       </c>
@@ -4310,8 +6398,14 @@
         <f t="shared" si="3"/>
         <v>5.8852511971060109E-5</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>0.87855877587003905</v>
+      </c>
+      <c r="N65">
+        <v>0.93811609576483102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.91099449700000001</v>
       </c>
@@ -4335,8 +6429,14 @@
         <f t="shared" ref="G66:G79" si="5">ABS(C66-A66)^2</f>
         <v>3.3928459514919693E-4</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>0.87531699504610605</v>
+      </c>
+      <c r="N66">
+        <v>0.93865362492934801</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.91977367399999999</v>
       </c>
@@ -4360,8 +6460,14 @@
         <f t="shared" si="5"/>
         <v>8.880321843917919E-5</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>0.87617387054636098</v>
+      </c>
+      <c r="N67">
+        <v>0.93905382886461697</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.933067808</v>
       </c>
@@ -4385,8 +6491,14 @@
         <f t="shared" si="5"/>
         <v>6.8363011123564506E-7</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>0.88063323294587303</v>
+      </c>
+      <c r="N68">
+        <v>0.93837805950337505</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.95212208099999995</v>
       </c>
@@ -4410,8 +6522,14 @@
         <f t="shared" si="5"/>
         <v>3.3698643484995206E-4</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <v>0.88653289150016001</v>
+      </c>
+      <c r="N69">
+        <v>0.93906803507841496</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.93059699100000004</v>
       </c>
@@ -4435,8 +6553,14 @@
         <f t="shared" si="5"/>
         <v>9.2270913041839873E-6</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M70">
+        <v>0.89109109553223498</v>
+      </c>
+      <c r="N70">
+        <v>0.94079470886383798</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.89937902300000006</v>
       </c>
@@ -4460,8 +6584,14 @@
         <f t="shared" si="5"/>
         <v>1.1644246638847226E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <v>0.89232035727759096</v>
+      </c>
+      <c r="N71">
+        <v>0.94132770495403495</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.90983941000000002</v>
       </c>
@@ -4485,8 +6615,14 @@
         <f t="shared" si="5"/>
         <v>5.5365940965119965E-4</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>0.89012478751900603</v>
+      </c>
+      <c r="N72">
+        <v>0.94185978348701804</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.92391890099999996</v>
       </c>
@@ -4510,8 +6646,14 @@
         <f t="shared" si="5"/>
         <v>8.6803574850499398E-5</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>0.886501042833306</v>
+      </c>
+      <c r="N73">
+        <v>0.94239094161375903</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.93967195199999998</v>
       </c>
@@ -4535,8 +6677,14 @@
         <f t="shared" si="5"/>
         <v>4.3163127478347458E-5</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M74">
+        <v>0.88436596152521296</v>
+      </c>
+      <c r="N74">
+        <v>0.94187028566589404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.93538478300000005</v>
       </c>
@@ -4560,8 +6708,14 @@
         <f t="shared" si="5"/>
         <v>5.8403620316746635E-6</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <v>0.88532010873896705</v>
+      </c>
+      <c r="N75">
+        <v>0.94213394286056995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.933353392</v>
       </c>
@@ -4585,8 +6739,14 @@
         <f t="shared" si="5"/>
         <v>2.7113536496679017E-7</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M76">
+        <v>0.888174116456105</v>
+      </c>
+      <c r="N76">
+        <v>0.94371141051799201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.94973285900000004</v>
       </c>
@@ -4610,8 +6770,14 @@
         <f t="shared" si="5"/>
         <v>2.9026537139758868E-4</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M77">
+        <v>0.88985600194064896</v>
+      </c>
+      <c r="N77">
+        <v>0.94450631616952896</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.93977904599999995</v>
       </c>
@@ -4635,8 +6801,14 @@
         <f t="shared" si="5"/>
         <v>5.2140544537333382E-5</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M78">
+        <v>0.88783509961768803</v>
+      </c>
+      <c r="N78">
+        <v>0.94503283105618197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.92457846499999996</v>
       </c>
@@ -4659,6 +6831,12 @@
       <c r="G79">
         <f t="shared" si="5"/>
         <v>6.1501192726129021E-5</v>
+      </c>
+      <c r="M79">
+        <v>0.88193239489415998</v>
+      </c>
+      <c r="N79">
+        <v>0.94555840906209299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>